<commit_message>
Updated Excel Schema Layout to reflect schema pushed to MongoDB
</commit_message>
<xml_diff>
--- a/Data Architecture/Schema.xlsx
+++ b/Data Architecture/Schema.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gallo\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gallo\Documents\GitHub\CS492\Data Architecture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6201E480-E2DE-47C1-BC66-209AE6BDB243}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49E41D74-2F9A-445C-9218-F6FC144663A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{E60CE7EA-1A50-4EBA-9840-04FDB930859F}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" firstSheet="1" activeTab="1" xr2:uid="{E60CE7EA-1A50-4EBA-9840-04FDB930859F}"/>
   </bookViews>
   <sheets>
     <sheet name="Menu Schema" sheetId="1" r:id="rId1"/>
-    <sheet name="Ingredients Schema" sheetId="2" r:id="rId2"/>
-    <sheet name="Portion Schema" sheetId="3" r:id="rId3"/>
-    <sheet name="Pizza Size Schema" sheetId="4" r:id="rId4"/>
-    <sheet name="MenuToIngredientsSchema" sheetId="5" r:id="rId5"/>
-    <sheet name="Menu to Price Schema" sheetId="10" r:id="rId6"/>
-    <sheet name="Order Review Schema" sheetId="11" r:id="rId7"/>
-    <sheet name="Order Details Schema" sheetId="12" r:id="rId8"/>
-    <sheet name="Payment Schema" sheetId="13" r:id="rId9"/>
+    <sheet name="Promotions Schema" sheetId="14" r:id="rId2"/>
+    <sheet name="Ingredients Schema" sheetId="2" r:id="rId3"/>
+    <sheet name="Portion Schema" sheetId="3" r:id="rId4"/>
+    <sheet name="Pizza Size Schema" sheetId="4" r:id="rId5"/>
+    <sheet name="MenuToIngredientsSchema" sheetId="5" r:id="rId6"/>
+    <sheet name="Menu to Price Schema" sheetId="10" r:id="rId7"/>
+    <sheet name="Order Review Schema" sheetId="11" r:id="rId8"/>
+    <sheet name="Order Details Schema" sheetId="12" r:id="rId9"/>
+    <sheet name="Payment Schema" sheetId="13" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="117">
   <si>
     <t>ItemID</t>
   </si>
@@ -350,6 +351,51 @@
   </si>
   <si>
     <t>OrderSubtotal</t>
+  </si>
+  <si>
+    <t>PromotionID</t>
+  </si>
+  <si>
+    <t>PromotionName</t>
+  </si>
+  <si>
+    <t>PromotionDescription</t>
+  </si>
+  <si>
+    <t>PromotionCriteria1</t>
+  </si>
+  <si>
+    <t>SystemAction</t>
+  </si>
+  <si>
+    <t>BOGO</t>
+  </si>
+  <si>
+    <t>BuyOneGetOne</t>
+  </si>
+  <si>
+    <t>Double the Deliciousness! Buy One Pizza, Get One Absolutely FREE!</t>
+  </si>
+  <si>
+    <t>FLOOR(COUNT(MAX(ItemNumber) / 2) &gt;= 1</t>
+  </si>
+  <si>
+    <t>SELECT TOP FLOOR(COUNT(MAX(ItemNumber) / 2)  Pizzas ORDER BY Itemprice SET ItemPrice = 0</t>
+  </si>
+  <si>
+    <t>LRG3TPN</t>
+  </si>
+  <si>
+    <t>Large 3 - Topping Pizza</t>
+  </si>
+  <si>
+    <t>Feast Like Royalty for Just $12.99! Get a Large 3-Topping Pizza!</t>
+  </si>
+  <si>
+    <t>WHERE [ItemID] Contains "1CP" and IngredientCount &gt;= 5</t>
+  </si>
+  <si>
+    <t>SELECT [ItemID] WHERE [ItemID] Contains "1CP" and IngredientCount &gt;= 5 SET ItemPrice = $12.99 + ($1.99 * [IngredientCount]  - 5)</t>
   </si>
 </sst>
 </file>
@@ -580,7 +626,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -653,9 +699,6 @@
     <xf numFmtId="10" fontId="4" fillId="3" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -677,31 +720,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -890,13 +908,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color rgb="FF44B3E1"/>
         </left>
@@ -909,12 +920,15 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -924,11 +938,29 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color rgb="FF000000"/>
+        <color theme="0"/>
         <name val="Aptos Narrow"/>
         <family val="2"/>
-        <scheme val="none"/>
+        <scheme val="minor"/>
       </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -967,86 +999,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1098,6 +1050,97 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
         <color theme="1"/>
         <name val="Aptos Narrow"/>
         <family val="2"/>
@@ -2030,7 +2073,45 @@
 </table>
 </file>
 
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5D4AAE15-43A7-4D6A-AF64-0B941669ED7C}" name="Table2" displayName="Table2" ref="B1:H2" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+  <autoFilter ref="B1:H2" xr:uid="{5D4AAE15-43A7-4D6A-AF64-0B941669ED7C}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{3E73D0B8-D07C-43A2-9814-6B5420657EF3}" name="OrderSubtotal" dataDxfId="6">
+      <calculatedColumnFormula>SUM(Table12[TotalItemPrice])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{C42B667A-7309-4D49-B8C2-CFA057CD5FE0}" name="Tax" dataDxfId="5" dataCellStyle="Percent">
+      <calculatedColumnFormula>SUM($H$2:$H$10)- (SUM($H$2:$H$10)*A2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{34F403C5-D38B-4157-A414-F047DDDF4E37}" name="Tax Amount" dataDxfId="4" dataCellStyle="Currency">
+      <calculatedColumnFormula>SUM(Table12[TotalItemPrice]) *Table12[[#This Row],[Tax]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{5BD567C5-8012-4709-93F5-65595D5F2F6B}" name="FinalTotal" dataDxfId="3">
+      <calculatedColumnFormula>Table12[[#This Row],[OrderSubtotal]]+Table12[[#This Row],[Tax Amount]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{736613BC-F5B4-40CC-96E9-D52A0F4C6926}" name="PaymentID" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{8D7DC34E-2BEB-4A97-93C8-8CFE85D1B7EF}" name="PaymentType" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{897562CA-50FF-4828-89E1-466FEFBD9BA1}" name="SubmittedDate" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{FC03C726-169F-4D02-84B7-242A59A7D278}" name="Table6" displayName="Table6" ref="A1:E3" totalsRowShown="0">
+  <autoFilter ref="A1:E3" xr:uid="{FC03C726-169F-4D02-84B7-242A59A7D278}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{E64E589C-C606-4FEE-8DF4-75D1916CA129}" name="PromotionID"/>
+    <tableColumn id="2" xr3:uid="{D027BE83-0707-4AEC-A7D7-C7682EDF6041}" name="PromotionName"/>
+    <tableColumn id="3" xr3:uid="{E74B734E-4DAE-45E8-B2F8-A603DEFCACC3}" name="PromotionDescription"/>
+    <tableColumn id="4" xr3:uid="{91A24508-2F10-43EB-B607-8236E1DCB26B}" name="PromotionCriteria1"/>
+    <tableColumn id="5" xr3:uid="{87184615-13E0-46C4-BF8E-AF7D30425008}" name="SystemAction"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{EA523E72-52F4-4671-98C5-28D46BABE2DB}" name="Table5" displayName="Table5" ref="A1:B15" totalsRowShown="0">
   <autoFilter ref="A1:B15" xr:uid="{EA523E72-52F4-4671-98C5-28D46BABE2DB}"/>
   <tableColumns count="2">
@@ -2041,7 +2122,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B5DB4573-F9E7-48A4-A3DE-4202E6F34671}" name="Table4" displayName="Table4" ref="A1:B5" totalsRowShown="0">
   <autoFilter ref="A1:B5" xr:uid="{B5DB4573-F9E7-48A4-A3DE-4202E6F34671}"/>
   <tableColumns count="2">
@@ -2052,7 +2133,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A3022EA4-6CF7-4C45-9C71-23EB3D590CC5}" name="Table3" displayName="Table3" ref="A1:D4" totalsRowShown="0">
   <autoFilter ref="A1:D4" xr:uid="{A3022EA4-6CF7-4C45-9C71-23EB3D590CC5}"/>
   <tableColumns count="4">
@@ -2065,7 +2146,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1772D3EA-E3AE-41B1-9F45-307B2DD6AE94}" name="Table1" displayName="Table1" ref="A1:S10" totalsRowShown="0">
   <autoFilter ref="A1:S10" xr:uid="{1772D3EA-E3AE-41B1-9F45-307B2DD6AE94}"/>
   <tableColumns count="19">
@@ -2099,7 +2180,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{A8CBA069-7D1F-48CA-9C52-0814D69045AD}" name="Table10" displayName="Table10" ref="A1:H10" totalsRowShown="0" headerRowDxfId="55" dataDxfId="53" headerRowBorderDxfId="54" tableBorderDxfId="52" totalsRowBorderDxfId="51">
   <autoFilter ref="A1:H10" xr:uid="{A8CBA069-7D1F-48CA-9C52-0814D69045AD}"/>
   <tableColumns count="8">
@@ -2126,7 +2207,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{7C30AC10-10C7-4B3C-ACC3-68365B4EFBD0}" name="Table1012" displayName="Table1012" ref="A1:L10" totalsRowShown="0" headerRowDxfId="42" dataDxfId="40" headerRowBorderDxfId="41" tableBorderDxfId="39" totalsRowBorderDxfId="38">
   <autoFilter ref="A1:L10" xr:uid="{A8CBA069-7D1F-48CA-9C52-0814D69045AD}"/>
   <tableColumns count="12">
@@ -2159,52 +2240,28 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{508A7AF8-D558-4763-8654-72D69D6CE90F}" name="Table12" displayName="Table12" ref="A1:L10" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24" tableBorderDxfId="23">
   <autoFilter ref="A1:L10" xr:uid="{508A7AF8-D558-4763-8654-72D69D6CE90F}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{37C9C776-33B1-4F6D-801A-51955FB00694}" name="OrderID" dataDxfId="22"/>
     <tableColumn id="2" xr3:uid="{E6404B9B-3168-480E-BF83-5CDC2E9CB3AB}" name="ItemNumber" dataDxfId="21"/>
     <tableColumn id="3" xr3:uid="{B685B8DD-03E9-4718-AC9E-E5C3FF2AB5A2}" name="ItemID" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{5BB59B26-98E4-4F40-9B5A-0EF825FD3229}" name="ItemName" dataDxfId="15"/>
-    <tableColumn id="11" xr3:uid="{34E783D9-8B27-46AE-89FA-D5FE4782EFE5}" name="TotalItemPrice" dataDxfId="14" dataCellStyle="Currency"/>
-    <tableColumn id="5" xr3:uid="{3DAA669C-453F-46F3-927D-618044CE7C04}" name="OrderSubtotal" dataDxfId="12">
+    <tableColumn id="4" xr3:uid="{5BB59B26-98E4-4F40-9B5A-0EF825FD3229}" name="ItemName" dataDxfId="19"/>
+    <tableColumn id="11" xr3:uid="{34E783D9-8B27-46AE-89FA-D5FE4782EFE5}" name="TotalItemPrice" dataDxfId="18" dataCellStyle="Currency"/>
+    <tableColumn id="5" xr3:uid="{3DAA669C-453F-46F3-927D-618044CE7C04}" name="OrderSubtotal" dataDxfId="17">
       <calculatedColumnFormula>SUM(Table12[TotalItemPrice])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{05D513FE-7128-47E3-961F-ABBAA09CDC59}" name="Tax" dataDxfId="19" dataCellStyle="Percent"/>
-    <tableColumn id="12" xr3:uid="{B073805E-9DEC-462B-A0A7-27C0B5CD2B05}" name="Tax Amount" dataDxfId="13" dataCellStyle="Currency">
+    <tableColumn id="6" xr3:uid="{05D513FE-7128-47E3-961F-ABBAA09CDC59}" name="Tax" dataDxfId="16" dataCellStyle="Percent"/>
+    <tableColumn id="12" xr3:uid="{B073805E-9DEC-462B-A0A7-27C0B5CD2B05}" name="Tax Amount" dataDxfId="15" dataCellStyle="Currency">
       <calculatedColumnFormula>SUM(Table12[TotalItemPrice]) *Table12[[#This Row],[Tax]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{4246F17B-1C01-4F14-87C1-5E009225B3F1}" name="FinalTotal" dataDxfId="11">
+    <tableColumn id="7" xr3:uid="{4246F17B-1C01-4F14-87C1-5E009225B3F1}" name="FinalTotal" dataDxfId="14">
       <calculatedColumnFormula>Table12[[#This Row],[OrderSubtotal]]+Table12[[#This Row],[Tax Amount]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{C16F91C9-045F-4855-B104-1445B33A12F3}" name="PaymentID" dataDxfId="18"/>
-    <tableColumn id="9" xr3:uid="{BC8C6664-86FA-4CE8-9C4B-D5343FE895E9}" name="PaymentType" dataDxfId="17"/>
-    <tableColumn id="10" xr3:uid="{6952ED59-4492-4EFB-BED7-4B54AAE195B3}" name="SubmittedDate" dataDxfId="16"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5D4AAE15-43A7-4D6A-AF64-0B941669ED7C}" name="Table2" displayName="Table2" ref="B1:H2" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="9" tableBorderDxfId="10" totalsRowBorderDxfId="8">
-  <autoFilter ref="B1:H2" xr:uid="{5D4AAE15-43A7-4D6A-AF64-0B941669ED7C}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{3E73D0B8-D07C-43A2-9814-6B5420657EF3}" name="OrderSubtotal" dataDxfId="7">
-      <calculatedColumnFormula>SUM(Table12[TotalItemPrice])</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="2" xr3:uid="{C42B667A-7309-4D49-B8C2-CFA057CD5FE0}" name="Tax" dataDxfId="6" dataCellStyle="Percent">
-      <calculatedColumnFormula>SUM($H$2:$H$10)- (SUM($H$2:$H$10)*A2)</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="3" xr3:uid="{34F403C5-D38B-4157-A414-F047DDDF4E37}" name="Tax Amount" dataDxfId="5" dataCellStyle="Currency">
-      <calculatedColumnFormula>SUM(Table12[TotalItemPrice]) *Table12[[#This Row],[Tax]]</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="4" xr3:uid="{5BD567C5-8012-4709-93F5-65595D5F2F6B}" name="FinalTotal" dataDxfId="4">
-      <calculatedColumnFormula>Table12[[#This Row],[OrderSubtotal]]+Table12[[#This Row],[Tax Amount]]</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="5" xr3:uid="{736613BC-F5B4-40CC-96E9-D52A0F4C6926}" name="PaymentID" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{8D7DC34E-2BEB-4A97-93C8-8CFE85D1B7EF}" name="PaymentType" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{897562CA-50FF-4828-89E1-466FEFBD9BA1}" name="SubmittedDate" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{C16F91C9-045F-4855-B104-1445B33A12F3}" name="PaymentID" dataDxfId="13"/>
+    <tableColumn id="9" xr3:uid="{BC8C6664-86FA-4CE8-9C4B-D5343FE895E9}" name="PaymentType" dataDxfId="12"/>
+    <tableColumn id="10" xr3:uid="{6952ED59-4492-4EFB-BED7-4B54AAE195B3}" name="SubmittedDate" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2529,7 +2586,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{515B8625-9870-42EC-A8C5-F0625474CD01}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
@@ -2675,7 +2732,159 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1A44538-D286-4209-923F-885E587986AC}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B6:B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="8" width="20.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="H1" s="38" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="25">
+        <v>1</v>
+      </c>
+      <c r="B2" s="37">
+        <f>SUM(Table12[TotalItemPrice])</f>
+        <v>148.91</v>
+      </c>
+      <c r="C2" s="27">
+        <v>0.08</v>
+      </c>
+      <c r="D2" s="26">
+        <f>SUM(Table12[TotalItemPrice]) *Table12[[#This Row],[Tax]]</f>
+        <v>11.912800000000001</v>
+      </c>
+      <c r="E2" s="28">
+        <f>Table12[[#This Row],[OrderSubtotal]]+Table12[[#This Row],[Tax Amount]]</f>
+        <v>160.8228</v>
+      </c>
+      <c r="F2" s="3">
+        <v>145</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="H2" s="29">
+        <v>45749</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E39E21A1-CA5C-4CF8-AAE0-700D728E4B4D}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="114.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFE9D601-C7F8-426A-8F01-330690FAD72D}">
   <dimension ref="A1:B15"/>
   <sheetViews>
@@ -2820,7 +3029,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6E6AC08-4ABF-472E-9778-460FF2497BE1}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -2882,7 +3091,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF608AA9-F532-42C5-A780-2FAE0409229A}">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -2961,7 +3170,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9308E57F-07B7-4C16-8249-6E35CCAF6630}">
   <dimension ref="A1:S10"/>
   <sheetViews>
@@ -3624,12 +3833,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{426267E2-D1F5-47CE-87C1-B999EF134463}">
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3968,7 +4177,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{278F732A-A123-40B2-ACE7-880A954D0183}">
   <dimension ref="A1:L10"/>
   <sheetViews>
@@ -4434,12 +4643,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{382DBEFB-123C-4FD6-B4DB-A07B3E875B71}">
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="J55" sqref="J55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4472,10 +4681,10 @@
       <c r="D1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="36" t="s">
         <v>99</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="F1" s="36" t="s">
         <v>101</v>
       </c>
       <c r="G1" s="22" t="s">
@@ -4511,10 +4720,10 @@
       <c r="D2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="38">
+      <c r="E2" s="37">
         <v>8.99</v>
       </c>
-      <c r="F2" s="38">
+      <c r="F2" s="37">
         <f>SUM(Table12[TotalItemPrice])</f>
         <v>148.91</v>
       </c>
@@ -4553,10 +4762,10 @@
       <c r="D3" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="38">
+      <c r="E3" s="37">
         <v>13.99</v>
       </c>
-      <c r="F3" s="38">
+      <c r="F3" s="37">
         <f>SUM(Table12[TotalItemPrice])</f>
         <v>148.91</v>
       </c>
@@ -4595,10 +4804,10 @@
       <c r="D4" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="38">
+      <c r="E4" s="37">
         <v>20.990000000000002</v>
       </c>
-      <c r="F4" s="38">
+      <c r="F4" s="37">
         <f>SUM(Table12[TotalItemPrice])</f>
         <v>148.91</v>
       </c>
@@ -4637,10 +4846,10 @@
       <c r="D5" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="38">
+      <c r="E5" s="37">
         <v>18.990000000000002</v>
       </c>
-      <c r="F5" s="38">
+      <c r="F5" s="37">
         <f>SUM(Table12[TotalItemPrice])</f>
         <v>148.91</v>
       </c>
@@ -4679,10 +4888,10 @@
       <c r="D6" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="38">
+      <c r="E6" s="37">
         <v>16.990000000000002</v>
       </c>
-      <c r="F6" s="38">
+      <c r="F6" s="37">
         <f>SUM(Table12[TotalItemPrice])</f>
         <v>148.91</v>
       </c>
@@ -4721,10 +4930,10 @@
       <c r="D7" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="38">
+      <c r="E7" s="37">
         <v>17.990000000000002</v>
       </c>
-      <c r="F7" s="38">
+      <c r="F7" s="37">
         <f>SUM(Table12[TotalItemPrice])</f>
         <v>148.91</v>
       </c>
@@ -4763,10 +4972,10 @@
       <c r="D8" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="38">
+      <c r="E8" s="37">
         <v>13.99</v>
       </c>
-      <c r="F8" s="38">
+      <c r="F8" s="37">
         <f>SUM(Table12[TotalItemPrice])</f>
         <v>148.91</v>
       </c>
@@ -4805,10 +5014,10 @@
       <c r="D9" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="38">
+      <c r="E9" s="37">
         <v>11.99</v>
       </c>
-      <c r="F9" s="38">
+      <c r="F9" s="37">
         <f>SUM(Table12[TotalItemPrice])</f>
         <v>148.91</v>
       </c>
@@ -4847,10 +5056,10 @@
       <c r="D10" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="38">
+      <c r="E10" s="37">
         <v>24.990000000000002</v>
       </c>
-      <c r="F10" s="38">
+      <c r="F10" s="37">
         <f>SUM(Table12[TotalItemPrice])</f>
         <v>148.91</v>
       </c>
@@ -4875,82 +5084,6 @@
         <v>45749</v>
       </c>
       <c r="M10"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1A44538-D286-4209-923F-885E587986AC}">
-  <dimension ref="A1:H2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B6:B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="8" width="20.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="B1" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="C1" s="22" t="s">
-        <v>86</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="E1" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="F1" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="G1" s="39" t="s">
-        <v>91</v>
-      </c>
-      <c r="H1" s="39" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="36">
-        <v>1</v>
-      </c>
-      <c r="B2" s="38">
-        <f>SUM(Table12[TotalItemPrice])</f>
-        <v>148.91</v>
-      </c>
-      <c r="C2" s="27">
-        <v>0.08</v>
-      </c>
-      <c r="D2" s="26">
-        <f>SUM(Table12[TotalItemPrice]) *Table12[[#This Row],[Tax]]</f>
-        <v>11.912800000000001</v>
-      </c>
-      <c r="E2" s="28">
-        <f>Table12[[#This Row],[OrderSubtotal]]+Table12[[#This Row],[Tax Amount]]</f>
-        <v>160.8228</v>
-      </c>
-      <c r="F2" s="3">
-        <v>145</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="H2" s="29">
-        <v>45749</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>